<commit_message>
Update satellite info files
</commit_message>
<xml_diff>
--- a/Hypothesis and Results.xlsx
+++ b/Hypothesis and Results.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\University\General\UG4\SCC421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B3CF70-461C-4858-B1EB-4A44D644D7D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D60D8B9-04AE-4896-9700-458785812693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Survey" sheetId="1" r:id="rId1"/>
+    <sheet name="Static Analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="170">
   <si>
     <t>Hypothesis</t>
   </si>
@@ -299,6 +301,649 @@
   </si>
   <si>
     <t>Below (9%)/Average (55%)/Above (37%)</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>No Issues</t>
+  </si>
+  <si>
+    <t>Semgrep (ci rules)</t>
+  </si>
+  <si>
+    <t>Semgrep (rc2-ci rules)</t>
+  </si>
+  <si>
+    <t>SonarQube</t>
+  </si>
+  <si>
+    <t>Semgrep (javascript rules)</t>
+  </si>
+  <si>
+    <t>Semgrep (java rules)</t>
+  </si>
+  <si>
+    <t>For-of loop recommended to replace for</t>
+  </si>
+  <si>
+    <t>SonarQube for .NET (Roslyn)</t>
+  </si>
+  <si>
+    <t>No issues</t>
+  </si>
+  <si>
+    <t>Repo</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Relevant Change</t>
+  </si>
+  <si>
+    <t>WinForms</t>
+  </si>
+  <si>
+    <t>Signal-Server</t>
+  </si>
+  <si>
+    <t>NPM-CLI</t>
+  </si>
+  <si>
+    <t>a6480ebfa7087d8cc935edc0f0b4be4ccafb8457</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/a6480ebfa7087d8cc935edc0f0b4be4ccafb8457</t>
+  </si>
+  <si>
+    <t>Instances</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/b9e82d49595fbd713f6c9ddaae4fc4ddf864db9d</t>
+  </si>
+  <si>
+    <t>b9e82d49595fbd713f6c9ddaae4fc4ddf864db9d</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Simple if-statement replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ternary</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If-statement null-check replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null coalesce</t>
+    </r>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/6a8192ea056babf51af1cf2210f8abe5545b6172</t>
+  </si>
+  <si>
+    <t>6a8192ea056babf51af1cf2210f8abe5545b6172</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Simple Get/Set block replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lambda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Simple method replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lambda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Simple getter/setter replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lambda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Simple getter/setter replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lamdba</t>
+    </r>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/265fe3166ba40c25b90d3a8c91ad8967b3fbf902</t>
+  </si>
+  <si>
+    <t>265fe3166ba40c25b90d3a8c91ad8967b3fbf902</t>
+  </si>
+  <si>
+    <t>2ca2e545efff8646f08208fb2b0bd9c46914655c</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/2ca2e545efff8646f08208fb2b0bd9c46914655c</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If-statement null-check replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null conditional</t>
+    </r>
+  </si>
+  <si>
+    <t>2cc0d749f52723152a985a6329f0da3945e2ce2e</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/2cc0d749f52723152a985a6329f0da3945e2ce2e</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lambda </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>replaced with simple getter/setter</t>
+    </r>
+  </si>
+  <si>
+    <t>96741c330c3767cb069c9cb3d4dbee4b0cec9a2f</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/96741c330c3767cb069c9cb3d4dbee4b0cec9a2f</t>
+  </si>
+  <si>
+    <t>69d8b0eb12daafe7a4e66850d8b0a259b428b0c0</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/69d8b0eb12daafe7a4e66850d8b0a259b428b0c0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ternary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> null-check replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null conditional</t>
+    </r>
+  </si>
+  <si>
+    <t>70f44374bae6b6fb31598a3cdc89049199a7f7f3</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/70f44374bae6b6fb31598a3cdc89049199a7f7f3</t>
+  </si>
+  <si>
+    <t>8d8794458589e518a3e52c4d03c749740a7dc5cc</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/8d8794458589e518a3e52c4d03c749740a7dc5cc</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ternary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">null-check replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null coalesce</t>
+    </r>
+  </si>
+  <si>
+    <t>5e664d06826d68abed14b3da363a11be1c44f361</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/5e664d06826d68abed14b3da363a11be1c44f361</t>
+  </si>
+  <si>
+    <t>825c984022eb3d4b544316b504863a2ea25a0292</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/825c984022eb3d4b544316b504863a2ea25a0292</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If-statement null-check replaced </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null coalesce</t>
+    </r>
+  </si>
+  <si>
+    <t>ff5b940cb019cc3336f0d8112603f50040f38d31</t>
+  </si>
+  <si>
+    <t>https://github.com/dotnet/winforms/commit/ff5b940cb019cc3336f0d8112603f50040f38d31</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ternary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">null-check replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null conditional</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Basic for-loop replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>foreach</t>
+    </r>
+  </si>
+  <si>
+    <t>f7e41edb947dad22e10eeaa2e68e6f44b4bfa747</t>
+  </si>
+  <si>
+    <t>https://github.com/checkstyle/checkstyle/commit/f7e41edb947dad22e10eeaa2e68e6f44b4bfa747</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ternary </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>replaced with if-statement</t>
+    </r>
+  </si>
+  <si>
+    <t>e6538f822f3fb690d01b3f27aabb6785d9732a29</t>
+  </si>
+  <si>
+    <t>https://github.com/checkstyle/checkstyle/commit/e6538f822f3fb690d01b3f27aabb6785d9732a29</t>
+  </si>
+  <si>
+    <t>85ba2a3dce39e73858d0f3df72c43804677c8c48</t>
+  </si>
+  <si>
+    <t>https://github.com/checkstyle/checkstyle/commit/85ba2a3dce39e73858d0f3df72c43804677c8c48</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Discrete operators replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>compound operator</t>
+    </r>
+  </si>
+  <si>
+    <t>95fa195d1cfdf581ee94a2d88ca6cec89b1ca3e9</t>
+  </si>
+  <si>
+    <t>https://github.com/checkstyle/checkstyle/commit/95fa195d1cfdf581ee94a2d88ca6cec89b1ca3e9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lambda </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>replaced method reference</t>
+    </r>
+  </si>
+  <si>
+    <t>3c2249b239cbfe002af3649f1f7c1f9ae61df3b1</t>
+  </si>
+  <si>
+    <t>https://github.com/checkstyle/checkstyle/commit/3c2249b239cbfe002af3649f1f7c1f9ae61df3b1</t>
+  </si>
+  <si>
+    <t>Checkstyle</t>
+  </si>
+  <si>
+    <t>a6fd1aa06c3968be2a7464c85414f79dc1235966</t>
+  </si>
+  <si>
+    <t>https://github.com/signalapp/Signal-Server/commit/a6fd1aa06c3968be2a7464c85414f79dc1235966</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Simple if-statement replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lambda</t>
+    </r>
+  </si>
+  <si>
+    <t>7e97d10ae1bf3ae43abb9fc89ce4080558582f34</t>
+  </si>
+  <si>
+    <t>https://github.com/signalapp/Signal-Server/commit/7e97d10ae1bf3ae43abb9fc89ce4080558582f34</t>
+  </si>
+  <si>
+    <t>a92d310b7e9e4c48b08f52785c2e3a6d52a82ad7</t>
+  </si>
+  <si>
+    <t>https://github.com/npm/cli/commit/a92d310b7e9e4c48b08f52785c2e3a6d52a82ad7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Foreach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>arrow function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for-of loop</t>
+    </r>
+  </si>
+  <si>
+    <t>d136c7ab61997608719a9d5eb1e27b1f4626c07b</t>
+  </si>
+  <si>
+    <t>https://github.com/npm/cli/commit/d136c7ab61997608719a9d5eb1e27b1f4626c07b</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Anonymous function replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>arrow function</t>
+    </r>
+  </si>
+  <si>
+    <t>8d71fcfd8555cdd33d4a407ef5e83814475f1d26</t>
+  </si>
+  <si>
+    <t>https://github.com/npm/cli/commit/8d71fcfd8555cdd33d4a407ef5e83814475f1d26</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For-in loop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">replaced forEach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anonymous function</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ForEach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>arrow function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for-of loop</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -330,12 +975,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -467,17 +1118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -485,22 +1130,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,516 +1474,516 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F55B0E-5E27-45E6-BFE1-1CD648DFFFDF}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="6" style="21" customWidth="1"/>
+    <col min="3" max="3" width="6" style="16" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" customWidth="1"/>
     <col min="5" max="5" width="126.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="23"/>
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="21" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="22" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="21" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="22" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="9" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="23"/>
+      <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="21" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="22" t="s">
+      <c r="A25" s="24"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="18"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="20"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="23"/>
+      <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="4" t="s">
+      <c r="A28" s="23"/>
+      <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="23"/>
+      <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="3" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="21" t="s">
+      <c r="A32" s="23"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="12" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="22" t="s">
+      <c r="A33" s="24"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="18"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="20"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="23"/>
+      <c r="B37" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="12" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="4" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -1334,12 +1991,12 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="21" t="s">
+      <c r="A40" s="23"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -1347,223 +2004,223 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="22" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="20"/>
+      <c r="C42" s="15"/>
       <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="4" t="s">
+      <c r="A43" s="23"/>
+      <c r="B43" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="4" t="s">
+      <c r="A44" s="23"/>
+      <c r="B44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="23"/>
+      <c r="B45" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="4" t="s">
+      <c r="A46" s="23"/>
+      <c r="B46" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="23"/>
+      <c r="B47" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="21" t="s">
+      <c r="A48" s="23"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="22" t="s">
+      <c r="A49" s="24"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="20"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="4" t="s">
+      <c r="A51" s="23"/>
+      <c r="B51" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="4" t="s">
+      <c r="A52" s="23"/>
+      <c r="B52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="23"/>
+      <c r="B53" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E53" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="4" t="s">
+      <c r="A54" s="23"/>
+      <c r="B54" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="3" t="s">
+      <c r="A55" s="23"/>
+      <c r="B55" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="21" t="s">
+      <c r="A56" s="23"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="12" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="22" t="s">
+      <c r="A57" s="24"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E57" s="18" t="s">
+      <c r="E57" s="13" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1576,13 +2233,13 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="B55:B57"/>
     <mergeCell ref="A50:A57"/>
     <mergeCell ref="A42:A49"/>
     <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A18:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1590,4 +2247,648 @@
     <ignoredError sqref="E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1BFC61-6803-462C-9E5C-A6B6C302E336}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="4" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5AF96C-27F4-4731-AB86-1CF4F35C7BCB}">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E28">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="28">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>166</v>
+      </c>
+      <c r="C46" t="s">
+        <v>167</v>
+      </c>
+      <c r="D46" t="s">
+        <v>168</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reassess results with finalised dataset
</commit_message>
<xml_diff>
--- a/Hypothesis and Results.xlsx
+++ b/Hypothesis and Results.xlsx
@@ -2,20 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\University\General\UG4\SCC421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A911DE45-9CC9-4138-B9FD-498A8B095F79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7C273C-B34F-467E-9D6C-3A24929F1452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
-    <sheet name="Static Analysis" sheetId="2" r:id="rId2"/>
-    <sheet name="Commits" sheetId="3" r:id="rId3"/>
+    <sheet name="Survey Freq." sheetId="4" r:id="rId2"/>
+    <sheet name="Static Analysis" sheetId="2" r:id="rId3"/>
+    <sheet name="Commits" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="194">
   <si>
     <t>Hypothesis</t>
   </si>
@@ -154,31 +155,10 @@
     <t>Average</t>
   </si>
   <si>
-    <t>93%</t>
-  </si>
-  <si>
-    <t>89%</t>
-  </si>
-  <si>
-    <t>70%</t>
-  </si>
-  <si>
-    <t>63%</t>
-  </si>
-  <si>
-    <t>81%</t>
-  </si>
-  <si>
     <t>Frequently/sometimes</t>
   </si>
   <si>
     <t>Frequently</t>
-  </si>
-  <si>
-    <t>Always/frequently</t>
-  </si>
-  <si>
-    <t>Frequently/sometimes, sole "never"</t>
   </si>
   <si>
     <t>Always/frequently/sometimes, wide spread</t>
@@ -237,69 +217,6 @@
     <t>Decreased</t>
   </si>
   <si>
-    <t>No change (57%)/Increase (36%)</t>
-  </si>
-  <si>
-    <t>No change (50%)/Decrease (28%)/Increase (22%)</t>
-  </si>
-  <si>
-    <t>Below (29%)/Average (29%)/Above (41%)</t>
-  </si>
-  <si>
-    <t>Below (33%)/Average (39%)/Above (28%)</t>
-  </si>
-  <si>
-    <t>Below (40%)/Average (50%)/Above (10%)</t>
-  </si>
-  <si>
-    <t>Below (25%)/Average (13%)/Above (63%)</t>
-  </si>
-  <si>
-    <t>Below (19%)/Average (6.25%)/Above (75%)</t>
-  </si>
-  <si>
-    <t>Below (18%)/Average (36%)/Above (46%)</t>
-  </si>
-  <si>
-    <t>Below (8%)/Average (50%)/Above (42%)</t>
-  </si>
-  <si>
-    <t>Below (50%)/Average (25%)/Above (25%)</t>
-  </si>
-  <si>
-    <t>Below (8%)/Average (42%)/Above (44%)</t>
-  </si>
-  <si>
-    <t>Below (22%)/Average (33%)/Above (44%)</t>
-  </si>
-  <si>
-    <t>Below (0%)/Average (25%)/Above (75%)</t>
-  </si>
-  <si>
-    <t>Below (17%)/Average (33%)/Above (50%)</t>
-  </si>
-  <si>
-    <t>Below (9%)/Average (27%)/Above (64%)</t>
-  </si>
-  <si>
-    <t>Below (0%)/Average (56%)/Above (44%)</t>
-  </si>
-  <si>
-    <t>Below (18%)/Average (47%)/Above (35%)</t>
-  </si>
-  <si>
-    <t>Below (0%)/Average (42%)/Above (58%)</t>
-  </si>
-  <si>
-    <t>Below (13%)/Average (53%)/Above (33%)</t>
-  </si>
-  <si>
-    <t>Below (13%)/Average (56%)/Above (31%)</t>
-  </si>
-  <si>
-    <t>Below (9%)/Average (55%)/Above (37%)</t>
-  </si>
-  <si>
     <t>Tool</t>
   </si>
   <si>
@@ -913,14 +830,176 @@
     <t>Lambda replaced with simple getter/setter</t>
   </si>
   <si>
-    <t>Result (REDO PERCENTAGES THEY ARE WRONG)</t>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>91%</t>
+  </si>
+  <si>
+    <t>78%</t>
+  </si>
+  <si>
+    <t>74%</t>
+  </si>
+  <si>
+    <t>96%</t>
+  </si>
+  <si>
+    <t>Always//sometimes, wide spread</t>
+  </si>
+  <si>
+    <t>Additional Notes</t>
+  </si>
+  <si>
+    <t>Top for style, Top for speed (small)</t>
+  </si>
+  <si>
+    <t>Top for clarity, Top for none</t>
+  </si>
+  <si>
+    <t>Top for simplicity</t>
+  </si>
+  <si>
+    <t>Bot for style</t>
+  </si>
+  <si>
+    <t>Bot for style, bot for clarity</t>
+  </si>
+  <si>
+    <t>Top for always</t>
+  </si>
+  <si>
+    <t>Top for never</t>
+  </si>
+  <si>
+    <t>Top for frequently (caution)</t>
+  </si>
+  <si>
+    <t>Second for frequently (caution)</t>
+  </si>
+  <si>
+    <t>Top for clarity</t>
+  </si>
+  <si>
+    <t>Top for style (small, 3-draw), top for none, bot for complexity (small)</t>
+  </si>
+  <si>
+    <t>Bot for clarity, top for complexity (small), top for speed (large)</t>
+  </si>
+  <si>
+    <t>Second bot for complexity (small)</t>
+  </si>
+  <si>
+    <t>Top for style (small, 3-draw), only OTHER marked for speed</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>1-14 years, 20+ years (okay then?)</t>
+  </si>
+  <si>
+    <t>Most: no change/don't know</t>
+  </si>
+  <si>
+    <t>Top for decrease</t>
+  </si>
+  <si>
+    <t>Top for no change (small)</t>
+  </si>
+  <si>
+    <t>Second top for no change (small)</t>
+  </si>
+  <si>
+    <t>Top for incease</t>
+  </si>
+  <si>
+    <t>No change (38%)/Increase (24%)/Don't know (33%)</t>
+  </si>
+  <si>
+    <t>Decrease (22%)/No change (39%)/Don't know (26%)</t>
+  </si>
+  <si>
+    <t>Top for above (small)</t>
+  </si>
+  <si>
+    <t>Second top for above (small)</t>
+  </si>
+  <si>
+    <t>Below (22%)/Average (17%)/Above (30%)/Don't know (30%)</t>
+  </si>
+  <si>
+    <t>Below (26%)/Average (26%)/Above (22%)/Don't know (26%)</t>
+  </si>
+  <si>
+    <t>Below (17%)/Average (17%)/Above (4%)/Don't know (61%)</t>
+  </si>
+  <si>
+    <t>Below (19%)/Average (5%)/Above (48%)/Don't know (29%)</t>
+  </si>
+  <si>
+    <t>Below (14%)/Average (5%)/Above (52%)/Don't know (29%)</t>
+  </si>
+  <si>
+    <t>Below (10%)/Average (19%)/Above (19%)/Don't know (52%)</t>
+  </si>
+  <si>
+    <t>Below (6%)/Average (33%)/Above (28%)/Don't know (33%)</t>
+  </si>
+  <si>
+    <t>Below (22%)/Average (11%)/Above (11%)/Don't know (56%)</t>
+  </si>
+  <si>
+    <t>Below (6%)/Average (29%)/Above (35 %)/Don't know (29%)</t>
+  </si>
+  <si>
+    <t>Below (12%)/Average (18%)/Above (24%)/Don't know (47%)</t>
+  </si>
+  <si>
+    <t>Below (0%)/Average (17%)/Above (48%)/Don't know (35%)</t>
+  </si>
+  <si>
+    <t>Below (13%)/Average (22%)/Above (39%)/Don't know (26%)</t>
+  </si>
+  <si>
+    <t>Below (4%)/Average (9%)/Above (30%)/Don't know (57%)</t>
+  </si>
+  <si>
+    <t>Below (0%)/Average (39%)/Above (30%)/Don't know (30%)</t>
+  </si>
+  <si>
+    <t>Below (13%)/Average (35%)/Above (26%)/Don't know (26%)</t>
+  </si>
+  <si>
+    <t>Below (0%)/Average (22%)/Above (30%)/Don't know (48%)</t>
+  </si>
+  <si>
+    <t>Below (9%)/Average (32%)/Above (23%)/Don't know (36%)</t>
+  </si>
+  <si>
+    <t>Below (9%)/Average (36%)/Above (23%)/Don't know (32%)</t>
+  </si>
+  <si>
+    <t>Below (5%)/Average (23%)/Above (18%)/Don't know (55%)</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -951,6 +1030,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -971,7 +1057,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1096,12 +1182,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1142,12 +1268,293 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="19">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
@@ -1187,7 +1594,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1FC5A51-46DF-46B2-959C-D5712AC5557A}" name="Table1" displayName="Table1" ref="A1:E45" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5825697-E1ED-4E07-9865-2F4D4F0590D2}" name="Table2" displayName="Table2" ref="C1:F20" headerRowDxfId="14" dataDxfId="15" headerRowBorderDxfId="0" tableBorderDxfId="16" headerRowCellStyle="Percent" dataCellStyle="Percent">
+  <autoFilter ref="C1:F20" xr:uid="{E8C21C78-32B4-4AAA-9115-83099526E1E2}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{50B45362-1D05-4263-8A4D-8990360CCD5C}" name="Below" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{F3B0CB81-C64E-4153-B382-603D308D537D}" name="Avg" dataDxfId="8" totalsRowDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{F2066787-B6BE-4D1D-B955-964ECFD591EE}" name="Above" dataDxfId="7" totalsRowDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{CABF1EF6-03E0-48E8-9FFF-0A6627D7AEAC}" name="DK" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="13" dataCellStyle="Percent"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1FC5A51-46DF-46B2-959C-D5712AC5557A}" name="Table1" displayName="Table1" ref="A1:E45" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17">
   <autoFilter ref="A1:E45" xr:uid="{E13F673D-13DB-474C-98DD-B9724CDF2869}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BF3B8E4F-CED7-4A11-A53F-BBAD6E082501}" name="Repo"/>
@@ -1497,22 +1922,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F55B0E-5E27-45E6-BFE1-1CD648DFFFDF}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="6" style="16" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
-    <col min="5" max="5" width="126.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="100.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="81.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1526,10 +1952,13 @@
         <v>0</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>2</v>
       </c>
@@ -1541,10 +1970,11 @@
         <v>15</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="3" t="s">
         <v>17</v>
@@ -1553,10 +1983,13 @@
         <v>16</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -1567,8 +2000,9 @@
       <c r="E4" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -1579,20 +2013,26 @@
       <c r="E5" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="28"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
       <c r="B7" s="25" t="s">
         <v>14</v>
@@ -1604,10 +2044,11 @@
         <v>21</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="28"/>
       <c r="B8" s="25"/>
       <c r="C8" s="16" t="s">
@@ -1617,10 +2058,11 @@
         <v>21</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="26"/>
       <c r="C9" s="17" t="s">
@@ -1630,10 +2072,11 @@
         <v>21</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="F9" s="33"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>4</v>
       </c>
@@ -1645,10 +2088,11 @@
         <v>15</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -1657,10 +2101,13 @@
         <v>16</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="28"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
@@ -1669,10 +2116,13 @@
         <v>22</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -1683,20 +2133,26 @@
       <c r="E13" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="25" t="s">
         <v>14</v>
@@ -1708,10 +2164,13 @@
         <v>21</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="25"/>
       <c r="C16" s="16" t="s">
@@ -1721,10 +2180,13 @@
         <v>21</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="26"/>
       <c r="C17" s="17" t="s">
@@ -1734,10 +2196,11 @@
         <v>21</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="F17" s="33"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>5</v>
       </c>
@@ -1749,10 +2212,11 @@
         <v>28</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="3" t="s">
         <v>17</v>
@@ -1761,10 +2225,13 @@
         <v>29</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
@@ -1773,10 +2240,13 @@
         <v>30</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="3" t="s">
         <v>12</v>
@@ -1785,10 +2255,13 @@
         <v>31</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="3" t="s">
         <v>13</v>
@@ -1797,10 +2270,11 @@
         <v>20</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="25" t="s">
         <v>14</v>
@@ -1812,10 +2286,11 @@
         <v>32</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="F23" s="30"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="25"/>
       <c r="C24" s="16" t="s">
@@ -1825,10 +2300,11 @@
         <v>33</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="F24" s="30"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
       <c r="B25" s="26"/>
       <c r="C25" s="17" t="s">
@@ -1836,8 +2312,9 @@
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="33"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>6</v>
       </c>
@@ -1849,10 +2326,11 @@
         <v>34</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="3" t="s">
         <v>17</v>
@@ -1861,10 +2339,11 @@
         <v>29</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F27" s="30"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
@@ -1875,8 +2354,11 @@
       <c r="E28" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="3" t="s">
         <v>12</v>
@@ -1885,22 +2367,26 @@
         <v>31</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="25" t="s">
         <v>14</v>
@@ -1912,10 +2398,11 @@
         <v>32</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="F31" s="30"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="28"/>
       <c r="B32" s="25"/>
       <c r="C32" s="16" t="s">
@@ -1925,10 +2412,11 @@
         <v>33</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="29"/>
       <c r="B33" s="26"/>
       <c r="C33" s="17" t="s">
@@ -1936,8 +2424,9 @@
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>7</v>
       </c>
@@ -1949,10 +2438,11 @@
         <v>15</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="3" t="s">
         <v>17</v>
@@ -1961,10 +2451,13 @@
         <v>35</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="28"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -1973,10 +2466,13 @@
         <v>18</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="3" t="s">
         <v>12</v>
@@ -1985,22 +2481,28 @@
         <v>36</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="25" t="s">
         <v>14</v>
@@ -2011,11 +2513,12 @@
       <c r="D39" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="F39" s="30"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
       <c r="B40" s="25"/>
       <c r="C40" s="16" t="s">
@@ -2024,11 +2527,12 @@
       <c r="D40" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="F40" s="30"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="29"/>
       <c r="B41" s="26"/>
       <c r="C41" s="17" t="s">
@@ -2038,10 +2542,11 @@
         <v>21</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="F41" s="33"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
         <v>8</v>
       </c>
@@ -2053,10 +2558,11 @@
         <v>37</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="F42" s="30"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="3" t="s">
         <v>17</v>
@@ -2065,10 +2571,11 @@
         <v>35</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="F43" s="30"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
       <c r="B44" s="3" t="s">
         <v>11</v>
@@ -2079,8 +2586,11 @@
       <c r="E44" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
       <c r="B45" s="3" t="s">
         <v>12</v>
@@ -2089,22 +2599,28 @@
         <v>31</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
       <c r="B46" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
       <c r="B47" s="25" t="s">
         <v>14</v>
@@ -2116,10 +2632,11 @@
         <v>38</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="F47" s="30"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
       <c r="B48" s="25"/>
       <c r="C48" s="16" t="s">
@@ -2129,10 +2646,11 @@
         <v>38</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="F48" s="30"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="29"/>
       <c r="B49" s="26"/>
       <c r="C49" s="17" t="s">
@@ -2142,10 +2660,11 @@
         <v>38</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="F49" s="33"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
         <v>9</v>
       </c>
@@ -2157,10 +2676,11 @@
         <v>37</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F50" s="30"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="28"/>
       <c r="B51" s="3" t="s">
         <v>17</v>
@@ -2169,22 +2689,24 @@
         <v>35</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="F51" s="30"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="28"/>
       <c r="B52" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="30"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
       <c r="B53" s="3" t="s">
         <v>12</v>
@@ -2193,22 +2715,28 @@
         <v>31</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="28"/>
       <c r="B54" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="28"/>
       <c r="B55" s="25" t="s">
         <v>14</v>
@@ -2220,10 +2748,11 @@
         <v>38</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="F55" s="30"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="28"/>
       <c r="B56" s="25"/>
       <c r="C56" s="16" t="s">
@@ -2233,10 +2762,11 @@
         <v>38</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="F56" s="30"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="29"/>
       <c r="B57" s="26"/>
       <c r="C57" s="17" t="s">
@@ -2246,11 +2776,58 @@
         <v>38</v>
       </c>
       <c r="E57" s="13" t="s">
-        <v>79</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="F57" s="33"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
+      <c r="D59" t="s">
+        <v>161</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="35"/>
+      <c r="C60" s="36"/>
+      <c r="D60" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="35"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="36"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="35"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="18">
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A34:A41"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A26:A33"/>
@@ -2259,26 +2836,442 @@
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A34:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5286011E-C5F6-4A28-86AD-8FBC1952AE38}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="A1:F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="39"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="40">
+        <v>0.22</v>
+      </c>
+      <c r="D2" s="41">
+        <v>0.17</v>
+      </c>
+      <c r="E2" s="41">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="42">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="43">
+        <v>0.26</v>
+      </c>
+      <c r="D3" s="44">
+        <v>0.26</v>
+      </c>
+      <c r="E3" s="44">
+        <v>0.22</v>
+      </c>
+      <c r="F3" s="45">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="38"/>
+      <c r="B4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="43">
+        <v>0.17</v>
+      </c>
+      <c r="D4" s="44">
+        <v>0.17</v>
+      </c>
+      <c r="E4" s="44">
+        <v>0.04</v>
+      </c>
+      <c r="F4" s="45">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="43">
+        <v>0.19</v>
+      </c>
+      <c r="D5" s="44">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="44">
+        <v>0.48</v>
+      </c>
+      <c r="F5" s="45">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="38"/>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="43">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D6" s="44">
+        <v>0.05</v>
+      </c>
+      <c r="E6" s="44">
+        <v>0.52</v>
+      </c>
+      <c r="F6" s="45">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="38"/>
+      <c r="B7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="44">
+        <v>0.19</v>
+      </c>
+      <c r="E7" s="44">
+        <v>0.19</v>
+      </c>
+      <c r="F7" s="45">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="43">
+        <v>0.06</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0.33</v>
+      </c>
+      <c r="E8" s="44">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F8" s="45">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="38"/>
+      <c r="B9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="43">
+        <v>0.22</v>
+      </c>
+      <c r="D9" s="44">
+        <v>0.11</v>
+      </c>
+      <c r="E9" s="44">
+        <v>0.11</v>
+      </c>
+      <c r="F9" s="45">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="43">
+        <v>0.06</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E10" s="44">
+        <v>0.35</v>
+      </c>
+      <c r="F10" s="45">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="43">
+        <v>0.12</v>
+      </c>
+      <c r="D11" s="44">
+        <v>0.18</v>
+      </c>
+      <c r="E11" s="44">
+        <v>0.24</v>
+      </c>
+      <c r="F11" s="45">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="43">
+        <v>0</v>
+      </c>
+      <c r="D12" s="44">
+        <v>0.17</v>
+      </c>
+      <c r="E12" s="44">
+        <v>0.48</v>
+      </c>
+      <c r="F12" s="45">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="43">
+        <v>0.13</v>
+      </c>
+      <c r="D13" s="44">
+        <v>0.22</v>
+      </c>
+      <c r="E13" s="44">
+        <v>0.39</v>
+      </c>
+      <c r="F13" s="45">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="D14" s="44">
+        <v>0.09</v>
+      </c>
+      <c r="E14" s="44">
+        <v>0.3</v>
+      </c>
+      <c r="F14" s="45">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="43">
+        <v>0</v>
+      </c>
+      <c r="D15" s="44">
+        <v>0.39</v>
+      </c>
+      <c r="E15" s="44">
+        <v>0.3</v>
+      </c>
+      <c r="F15" s="45">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="43">
+        <v>0.13</v>
+      </c>
+      <c r="D16" s="44">
+        <v>0.35</v>
+      </c>
+      <c r="E16" s="44">
+        <v>0.26</v>
+      </c>
+      <c r="F16" s="45">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="43">
+        <v>0</v>
+      </c>
+      <c r="D17" s="44">
+        <v>0.22</v>
+      </c>
+      <c r="E17" s="44">
+        <v>0.3</v>
+      </c>
+      <c r="F17" s="45">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="43">
+        <v>0.09</v>
+      </c>
+      <c r="D18" s="44">
+        <v>0.32</v>
+      </c>
+      <c r="E18" s="44">
+        <v>0.23</v>
+      </c>
+      <c r="F18" s="45">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="43">
+        <v>0.09</v>
+      </c>
+      <c r="D19" s="44">
+        <v>0.36</v>
+      </c>
+      <c r="E19" s="44">
+        <v>0.23</v>
+      </c>
+      <c r="F19" s="45">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="46">
+        <v>0.05</v>
+      </c>
+      <c r="D20" s="47">
+        <v>0.23</v>
+      </c>
+      <c r="E20" s="47">
+        <v>0.18</v>
+      </c>
+      <c r="F20" s="48">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:F20">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>MAX(C$2:C$20)=C2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>MIN(C$2:C$20)=C2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B20">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>MAX($C2:$F2)&lt;&gt;$F2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1BFC61-6803-462C-9E5C-A6B6C302E336}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2290,82 +3283,82 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2374,7 +3367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5AF96C-27F4-4731-AB86-1CF4F35C7BCB}">
   <dimension ref="A1:E45"/>
   <sheetViews>
@@ -2393,33 +3386,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -2427,7 +3420,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -2435,13 +3428,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -2449,7 +3442,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2457,7 +3450,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -2465,7 +3458,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2473,13 +3466,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E8">
         <v>108</v>
@@ -2487,7 +3480,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -2495,7 +3488,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -2503,13 +3496,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -2517,7 +3510,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E12">
         <v>8</v>
@@ -2525,13 +3518,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E13">
         <v>28</v>
@@ -2539,7 +3532,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -2547,7 +3540,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -2555,7 +3548,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -2563,7 +3556,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E17">
         <v>25</v>
@@ -2571,13 +3564,13 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="E18">
         <v>42</v>
@@ -2585,7 +3578,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E19">
         <v>18</v>
@@ -2593,7 +3586,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D20" s="24" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="E20" s="24">
         <v>19</v>
@@ -2601,7 +3594,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -2609,13 +3602,13 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="D22" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E22">
         <v>3</v>
@@ -2623,7 +3616,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E23">
         <v>124</v>
@@ -2631,7 +3624,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2639,13 +3632,13 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="E25">
         <v>20</v>
@@ -2653,13 +3646,13 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
       <c r="E26">
         <v>46</v>
@@ -2667,13 +3660,13 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E27">
         <v>39</v>
@@ -2681,13 +3674,13 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="E28">
         <v>36</v>
@@ -2695,13 +3688,13 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="C29" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="E29" s="23">
         <v>441</v>
@@ -2709,7 +3702,7 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="E30">
         <v>441</v>
@@ -2717,13 +3710,13 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -2731,7 +3724,7 @@
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="E32">
         <v>12</v>
@@ -2739,7 +3732,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="E33">
         <v>5</v>
@@ -2747,7 +3740,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -2755,7 +3748,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -2763,16 +3756,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="E36" s="24">
         <v>1</v>
@@ -2780,13 +3773,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="E37">
         <v>6</v>
@@ -2794,13 +3787,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="C38" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -2808,13 +3801,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="D39" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="E39">
         <v>2</v>
@@ -2822,13 +3815,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="C40" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="E40">
         <v>3</v>
@@ -2836,16 +3829,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2853,16 +3846,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -2870,13 +3863,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="E43">
         <v>9</v>
@@ -2884,7 +3877,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="E44">
         <v>3</v>
@@ -2892,13 +3885,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="D45" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="E45">
         <v>2</v>

</xml_diff>

<commit_message>
Nearly finished survey stuff
</commit_message>
<xml_diff>
--- a/Hypothesis and Results.xlsx
+++ b/Hypothesis and Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\University\General\UG4\SCC421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014CF3A9-E923-4FC1-9F32-F7D6F6889A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A146C0-A4DF-4A01-9425-72CCB5CCAC6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="214">
   <si>
     <t>Hypothesis</t>
   </si>
@@ -1024,12 +1024,30 @@
   <si>
     <t>Fitment area</t>
   </si>
+  <si>
+    <t>Decreased Performance</t>
+  </si>
+  <si>
+    <t>Increased Performance</t>
+  </si>
+  <si>
+    <t>Don't Know</t>
+  </si>
+  <si>
+    <t>Below Average</t>
+  </si>
+  <si>
+    <t>Above Average</t>
+  </si>
+  <si>
+    <t>Don't know</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1084,6 +1102,14 @@
     <font>
       <sz val="28"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1358,13 +1384,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1406,6 +1433,17 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1427,52 +1465,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
@@ -1716,8 +1724,37 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF546E7A"/>
+      <color rgb="FF43A047"/>
+      <color rgb="FFFF9933"/>
+      <color rgb="FFE53935"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2131,6 +2168,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-0794-47DF-871A-6877D2F99298}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2150,6 +2192,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-0794-47DF-871A-6877D2F99298}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2169,6 +2216,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0794-47DF-871A-6877D2F99298}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2188,6 +2240,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-0794-47DF-871A-6877D2F99298}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -2207,6 +2264,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-0794-47DF-871A-6877D2F99298}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:numFmt formatCode="0.0%" sourceLinked="0"/>
@@ -2428,6 +2490,672 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8CB0-4297-9744-193B19D6D45A}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9933"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-B185-42C1-A66F-68CBDE57259D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B185-42C1-A66F-68CBDE57259D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="546E7A"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B185-42C1-A66F-68CBDE57259D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:sysClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Additional Vis'!$M$2:$P$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Decreased Performance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>No change</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Increased Performance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Don't Know</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Additional Vis'!$M$3:$P$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B185-42C1-A66F-68CBDE57259D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E53935"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E53935"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-5C36-4EDE-80B5-44CE938ACD12}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9933"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5C36-4EDE-80B5-44CE938ACD12}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="43A047"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-5C36-4EDE-80B5-44CE938ACD12}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="546E7A"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5C36-4EDE-80B5-44CE938ACD12}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Additional Vis'!$R$2:$U$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Below Average</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Average</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Above Average</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Don't know</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Additional Vis'!$R$3:$U$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C36-4EDE-80B5-44CE938ACD12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79382393735433709"/>
+          <c:y val="1.4199198732879902E-2"/>
+          <c:w val="0.19651697274488772"/>
+          <c:h val="0.2070727662349762"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2508,6 +3236,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
@@ -3710,20 +4518,1222 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>167447</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>121224</xdr:rowOff>
+      <xdr:rowOff>36884</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>437031</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>470585</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:rowOff>93773</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3751,15 +5761,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>59275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>82627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>487700</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>115303</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3784,11 +5794,83 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>90766</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>167809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>549088</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1376</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{700289A8-E7C8-4D45-A19D-7839D608D06F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>68353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>502228</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>91655</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0391AC69-A2C6-45AB-A583-DDAF24389D38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5825697-E1ED-4E07-9865-2F4D4F0590D2}" name="Table2" displayName="Table2" ref="C1:F20" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" headerRowCellStyle="Percent" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F5825697-E1ED-4E07-9865-2F4D4F0590D2}" name="Table2" displayName="Table2" ref="C1:F20" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" headerRowCellStyle="Percent" dataCellStyle="Percent">
   <autoFilter ref="C1:F20" xr:uid="{E8C21C78-32B4-4AAA-9115-83099526E1E2}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3796,17 +5878,17 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{50B45362-1D05-4263-8A4D-8990360CCD5C}" name="Below" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="2" xr3:uid="{F3B0CB81-C64E-4153-B382-603D308D537D}" name="Avg" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{F2066787-B6BE-4D1D-B955-964ECFD591EE}" name="Above" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{CABF1EF6-03E0-48E8-9FFF-0A6627D7AEAC}" name="DK" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{50B45362-1D05-4263-8A4D-8990360CCD5C}" name="Below" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{F3B0CB81-C64E-4153-B382-603D308D537D}" name="Avg" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{F2066787-B6BE-4D1D-B955-964ECFD591EE}" name="Above" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{CABF1EF6-03E0-48E8-9FFF-0A6627D7AEAC}" name="DK" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1FC5A51-46DF-46B2-959C-D5712AC5557A}" name="Table1" displayName="Table1" ref="A1:E43" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1FC5A51-46DF-46B2-959C-D5712AC5557A}" name="Table1" displayName="Table1" ref="A1:E43" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
   <autoFilter ref="A1:E43" xr:uid="{E13F673D-13DB-474C-98DD-B9724CDF2869}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BF3B8E4F-CED7-4A11-A53F-BBAD6E082501}" name="Repo"/>
@@ -4119,7 +6201,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A42" sqref="A42:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4153,7 +6235,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="56" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -4169,7 +6251,7 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -4184,7 +6266,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -4197,7 +6279,7 @@
       <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -4212,7 +6294,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -4227,8 +6309,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="57"/>
+      <c r="B7" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -4243,8 +6325,8 @@
       <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
@@ -4257,8 +6339,8 @@
       <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="17" t="s">
         <v>27</v>
       </c>
@@ -4271,7 +6353,7 @@
       <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="56" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4287,7 +6369,7 @@
       <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
@@ -4302,7 +6384,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -4317,7 +6399,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
@@ -4332,7 +6414,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
@@ -4347,8 +6429,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="57"/>
+      <c r="B15" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -4365,8 +6447,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="16" t="s">
         <v>26</v>
       </c>
@@ -4381,8 +6463,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="17" t="s">
         <v>27</v>
       </c>
@@ -4395,7 +6477,7 @@
       <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="56" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -4411,7 +6493,7 @@
       <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
@@ -4426,7 +6508,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -4441,7 +6523,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
@@ -4456,7 +6538,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
@@ -4469,8 +6551,8 @@
       <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
-      <c r="B23" s="43" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -4485,8 +6567,8 @@
       <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="43"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="16" t="s">
         <v>26</v>
       </c>
@@ -4499,8 +6581,8 @@
       <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="44"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="17" t="s">
         <v>27</v>
       </c>
@@ -4509,7 +6591,7 @@
       <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="56" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -4525,7 +6607,7 @@
       <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
@@ -4538,7 +6620,7 @@
       <c r="F27" s="23"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -4553,7 +6635,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
@@ -4568,7 +6650,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="3" t="s">
         <v>13</v>
       </c>
@@ -4581,8 +6663,8 @@
       <c r="F30" s="23"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="43" t="s">
+      <c r="A31" s="57"/>
+      <c r="B31" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -4597,8 +6679,8 @@
       <c r="F31" s="23"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="46"/>
-      <c r="B32" s="43"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="16" t="s">
         <v>26</v>
       </c>
@@ -4611,8 +6693,8 @@
       <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="17" t="s">
         <v>27</v>
       </c>
@@ -4621,7 +6703,7 @@
       <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="56" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -4637,7 +6719,7 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
+      <c r="A35" s="57"/>
       <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
@@ -4652,7 +6734,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
+      <c r="A36" s="57"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -4667,7 +6749,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
+      <c r="A37" s="57"/>
       <c r="B37" s="3" t="s">
         <v>12</v>
       </c>
@@ -4682,7 +6764,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="57"/>
       <c r="B38" s="3" t="s">
         <v>13</v>
       </c>
@@ -4697,8 +6779,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
-      <c r="B39" s="43" t="s">
+      <c r="A39" s="57"/>
+      <c r="B39" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -4713,8 +6795,8 @@
       <c r="F39" s="23"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="46"/>
-      <c r="B40" s="43"/>
+      <c r="A40" s="57"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="16" t="s">
         <v>26</v>
       </c>
@@ -4727,8 +6809,8 @@
       <c r="F40" s="23"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="44"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="17" t="s">
         <v>27</v>
       </c>
@@ -4741,7 +6823,7 @@
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="56" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -4757,7 +6839,7 @@
       <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="46"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="3" t="s">
         <v>17</v>
       </c>
@@ -4770,7 +6852,7 @@
       <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="46"/>
+      <c r="A44" s="57"/>
       <c r="B44" s="3" t="s">
         <v>11</v>
       </c>
@@ -4785,7 +6867,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="46"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="3" t="s">
         <v>12</v>
       </c>
@@ -4800,7 +6882,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="46"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="3" t="s">
         <v>13</v>
       </c>
@@ -4815,8 +6897,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="46"/>
-      <c r="B47" s="43" t="s">
+      <c r="A47" s="57"/>
+      <c r="B47" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="16" t="s">
@@ -4831,8 +6913,8 @@
       <c r="F47" s="23"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
-      <c r="B48" s="43"/>
+      <c r="A48" s="57"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="16" t="s">
         <v>26</v>
       </c>
@@ -4845,8 +6927,8 @@
       <c r="F48" s="23"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
-      <c r="B49" s="44"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="17" t="s">
         <v>27</v>
       </c>
@@ -4859,7 +6941,7 @@
       <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="56" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -4875,7 +6957,7 @@
       <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="46"/>
+      <c r="A51" s="57"/>
       <c r="B51" s="3" t="s">
         <v>17</v>
       </c>
@@ -4888,7 +6970,7 @@
       <c r="F51" s="23"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="46"/>
+      <c r="A52" s="57"/>
       <c r="B52" s="3" t="s">
         <v>11</v>
       </c>
@@ -4901,7 +6983,7 @@
       <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="46"/>
+      <c r="A53" s="57"/>
       <c r="B53" s="3" t="s">
         <v>12</v>
       </c>
@@ -4916,7 +6998,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
+      <c r="A54" s="57"/>
       <c r="B54" s="3" t="s">
         <v>13</v>
       </c>
@@ -4931,8 +7013,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="46"/>
-      <c r="B55" s="43" t="s">
+      <c r="A55" s="57"/>
+      <c r="B55" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="16" t="s">
@@ -4947,8 +7029,8 @@
       <c r="F55" s="23"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="46"/>
-      <c r="B56" s="43"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="16" t="s">
         <v>26</v>
       </c>
@@ -4961,8 +7043,8 @@
       <c r="F56" s="23"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
-      <c r="B57" s="44"/>
+      <c r="A57" s="58"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="17" t="s">
         <v>27</v>
       </c>
@@ -4975,11 +7057,11 @@
       <c r="F57" s="26"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="41" t="s">
+      <c r="A59" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="B59" s="41"/>
-      <c r="C59" s="42"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="53"/>
       <c r="D59" t="s">
         <v>160</v>
       </c>
@@ -4988,11 +7070,11 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B60" s="41"/>
-      <c r="C60" s="42"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="53"/>
       <c r="D60" t="s">
         <v>162</v>
       </c>
@@ -5001,14 +7083,14 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="42"/>
+      <c r="A61" s="52"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="53"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="41"/>
-      <c r="B62" s="41"/>
-      <c r="C62" s="42"/>
+      <c r="A62" s="52"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -5038,15 +7120,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA9E807-1B68-4F99-A999-3003C8845019}">
-  <dimension ref="A2:N47"/>
+  <dimension ref="A2:U47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>196</v>
       </c>
@@ -5077,8 +7159,32 @@
       <c r="K2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>208</v>
+      </c>
+      <c r="N2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P2" t="s">
+        <v>210</v>
+      </c>
+      <c r="R2" t="s">
+        <v>211</v>
+      </c>
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" t="s">
+        <v>212</v>
+      </c>
+      <c r="U2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>22</v>
       </c>
@@ -5109,25 +7215,49 @@
       <c r="K3">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="53"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="54"/>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>90</v>
+      </c>
+      <c r="O3">
+        <v>16</v>
+      </c>
+      <c r="P3">
+        <v>33</v>
+      </c>
+      <c r="R3">
+        <v>44</v>
+      </c>
+      <c r="S3">
+        <v>89</v>
+      </c>
+      <c r="T3">
+        <v>116</v>
+      </c>
+      <c r="U3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="45"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -5139,10 +7269,10 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="55"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="54"/>
+      <c r="N21" s="47"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="46"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -5154,10 +7284,10 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="55"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="54"/>
+      <c r="N22" s="47"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="46"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -5169,10 +7299,10 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="55"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="54"/>
+      <c r="N23" s="47"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="46"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -5184,10 +7314,10 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="55"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="54"/>
+      <c r="N24" s="47"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="46"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -5199,10 +7329,10 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="55"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="54"/>
+      <c r="N25" s="47"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="46"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -5214,10 +7344,10 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="55"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="54"/>
+      <c r="N26" s="47"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="46"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -5229,10 +7359,10 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="55"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" s="54"/>
+      <c r="N27" s="47"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="46"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -5244,10 +7374,10 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="55"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="54"/>
+      <c r="N28" s="47"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="46"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="59" t="s">
@@ -5261,10 +7391,10 @@
       <c r="K29" s="59"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="55"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B30" s="54"/>
+      <c r="N29" s="47"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="46"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="59"/>
@@ -5276,10 +7406,11 @@
       <c r="K30" s="59"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="55"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="54"/>
+      <c r="N30" s="47"/>
+      <c r="T30" s="61"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="46"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="59"/>
@@ -5291,10 +7422,10 @@
       <c r="K31" s="59"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="55"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="54"/>
+      <c r="N31" s="47"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="46"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="59"/>
@@ -5306,10 +7437,10 @@
       <c r="K32" s="59"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="55"/>
+      <c r="N32" s="47"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="54"/>
+      <c r="B33" s="46"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="59"/>
@@ -5321,10 +7452,10 @@
       <c r="K33" s="59"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
-      <c r="N33" s="55"/>
+      <c r="N33" s="47"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="54"/>
+      <c r="B34" s="46"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="59"/>
@@ -5336,10 +7467,10 @@
       <c r="K34" s="59"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="55"/>
+      <c r="N34" s="47"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="54"/>
+      <c r="B35" s="46"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="59"/>
@@ -5351,10 +7482,10 @@
       <c r="K35" s="59"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
-      <c r="N35" s="55"/>
+      <c r="N35" s="47"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="54"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="59"/>
@@ -5366,10 +7497,10 @@
       <c r="K36" s="59"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
-      <c r="N36" s="55"/>
+      <c r="N36" s="47"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="54"/>
+      <c r="B37" s="46"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="59"/>
@@ -5381,10 +7512,10 @@
       <c r="K37" s="59"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
-      <c r="N37" s="55"/>
+      <c r="N37" s="47"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="54"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -5396,10 +7527,10 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-      <c r="N38" s="55"/>
+      <c r="N38" s="47"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="54"/>
+      <c r="B39" s="46"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
@@ -5411,10 +7542,10 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
-      <c r="N39" s="55"/>
+      <c r="N39" s="47"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="54"/>
+      <c r="B40" s="46"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -5426,10 +7557,10 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
-      <c r="N40" s="55"/>
+      <c r="N40" s="47"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="54"/>
+      <c r="B41" s="46"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -5441,10 +7572,10 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-      <c r="N41" s="55"/>
+      <c r="N41" s="47"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="54"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -5456,10 +7587,10 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
-      <c r="N42" s="55"/>
+      <c r="N42" s="47"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="54"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -5471,10 +7602,10 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-      <c r="N43" s="55"/>
+      <c r="N43" s="47"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="54"/>
+      <c r="B44" s="46"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -5486,10 +7617,10 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
-      <c r="N44" s="55"/>
+      <c r="N44" s="47"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="54"/>
+      <c r="B45" s="46"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -5501,10 +7632,10 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
-      <c r="N45" s="55"/>
+      <c r="N45" s="47"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="54"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -5516,29 +7647,30 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
-      <c r="N46" s="55"/>
+      <c r="N46" s="47"/>
     </row>
     <row r="47" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="56"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="57"/>
-      <c r="M47" s="57"/>
-      <c r="N47" s="58"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E29:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5582,7 +7714,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="60" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -5602,7 +7734,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="8" t="s">
         <v>26</v>
       </c>
@@ -5620,7 +7752,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
@@ -5638,7 +7770,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="60" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -5658,7 +7790,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="8" t="s">
         <v>26</v>
       </c>
@@ -5676,7 +7808,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="8" t="s">
         <v>27</v>
       </c>
@@ -5694,7 +7826,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="60" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -5714,7 +7846,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
@@ -5732,7 +7864,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="60" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -5752,7 +7884,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
@@ -5770,7 +7902,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="60" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -5790,7 +7922,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
@@ -5808,7 +7940,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="8" t="s">
         <v>27</v>
       </c>
@@ -5826,7 +7958,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="60" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -5846,7 +7978,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
@@ -5864,7 +7996,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="8" t="s">
         <v>27</v>
       </c>
@@ -5882,7 +8014,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="60" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -5902,7 +8034,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
@@ -5920,7 +8052,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="8" t="s">
         <v>27</v>
       </c>
@@ -5948,15 +8080,15 @@
     <mergeCell ref="A12:A14"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:F20">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>MIN(C$2:C$20)=C2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>MAX(C$2:C$20)=C2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B20">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>MAX($C2:$F2)&lt;&gt;$F2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6071,7 +8203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5AF96C-27F4-4731-AB86-1CF4F35C7BCB}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -6139,10 +8271,10 @@
       <c r="C4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E4" s="41">
         <v>10</v>
       </c>
       <c r="G4" t="s">
@@ -6150,18 +8282,18 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="49">
+      <c r="E6" s="41">
         <v>3</v>
       </c>
     </row>
@@ -6270,26 +8402,26 @@
       <c r="C17" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="41">
         <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="E18" s="60">
+      <c r="E18" s="51">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="41">
         <v>2</v>
       </c>
     </row>
@@ -6457,10 +8589,10 @@
       <c r="C34" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="50">
+      <c r="E34" s="42">
         <v>1</v>
       </c>
     </row>
@@ -6471,10 +8603,10 @@
       <c r="C35" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="E35" s="49">
+      <c r="E35" s="41">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to working materials
</commit_message>
<xml_diff>
--- a/Hypothesis and Results.xlsx
+++ b/Hypothesis and Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\University\General\UG4\SCC421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042107C8-632F-40AE-8B6B-FEA66E57D86E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95237C1-D5BF-4B9A-9B34-99CAAEE627B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -1445,6 +1445,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1459,12 +1465,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3156,6 +3156,310 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E53935"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="E53935"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C896-4EF6-A4E6-C5BD224B1004}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9933"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C896-4EF6-A4E6-C5BD224B1004}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="43A047"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C896-4EF6-A4E6-C5BD224B1004}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="0.0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Additional Vis'!$R$2:$T$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Below Average</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Average</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Above Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Additional Vis'!$R$3:$T$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-C896-4EF6-A4E6-C5BD224B1004}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79382393735433709"/>
+          <c:y val="1.4199198732879902E-2"/>
+          <c:w val="0.19651697274488772"/>
+          <c:h val="0.2070727662349762"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3316,6 +3620,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
@@ -5120,6 +5464,607 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5861,6 +6806,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>20265</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D8C479-A102-4644-8761-8BDDED633A91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6200,8 +7183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F55B0E-5E27-45E6-BFE1-1CD648DFFFDF}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:A49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6235,7 +7218,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -6251,7 +7234,7 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -6266,7 +7249,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -6279,7 +7262,7 @@
       <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -6294,7 +7277,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -6309,8 +7292,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="53" t="s">
+      <c r="A7" s="58"/>
+      <c r="B7" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -6325,8 +7308,8 @@
       <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="53"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
@@ -6339,8 +7322,8 @@
       <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="54"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="17" t="s">
         <v>27</v>
       </c>
@@ -6353,7 +7336,7 @@
       <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="57" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -6369,7 +7352,7 @@
       <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="58"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
@@ -6384,7 +7367,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="58"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -6399,7 +7382,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
@@ -6414,7 +7397,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
@@ -6429,8 +7412,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="53" t="s">
+      <c r="A15" s="58"/>
+      <c r="B15" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -6447,8 +7430,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="53"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="16" t="s">
         <v>26</v>
       </c>
@@ -6463,8 +7446,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="17" t="s">
         <v>27</v>
       </c>
@@ -6477,7 +7460,7 @@
       <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="57" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -6493,7 +7476,7 @@
       <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
@@ -6508,7 +7491,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -6523,7 +7506,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
@@ -6538,7 +7521,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
@@ -6551,8 +7534,8 @@
       <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="53" t="s">
+      <c r="A23" s="58"/>
+      <c r="B23" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -6567,8 +7550,8 @@
       <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="55"/>
       <c r="C24" s="16" t="s">
         <v>26</v>
       </c>
@@ -6581,8 +7564,8 @@
       <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="56"/>
       <c r="C25" s="17" t="s">
         <v>27</v>
       </c>
@@ -6591,7 +7574,7 @@
       <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="57" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -6607,7 +7590,7 @@
       <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
@@ -6620,7 +7603,7 @@
       <c r="F27" s="23"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
+      <c r="A28" s="58"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -6635,7 +7618,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
+      <c r="A29" s="58"/>
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
@@ -6650,7 +7633,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
+      <c r="A30" s="58"/>
       <c r="B30" s="3" t="s">
         <v>13</v>
       </c>
@@ -6663,8 +7646,8 @@
       <c r="F30" s="23"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="53" t="s">
+      <c r="A31" s="58"/>
+      <c r="B31" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -6679,8 +7662,8 @@
       <c r="F31" s="23"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
-      <c r="B32" s="53"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="16" t="s">
         <v>26</v>
       </c>
@@ -6693,8 +7676,8 @@
       <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="57"/>
-      <c r="B33" s="54"/>
+      <c r="A33" s="59"/>
+      <c r="B33" s="56"/>
       <c r="C33" s="17" t="s">
         <v>27</v>
       </c>
@@ -6703,7 +7686,7 @@
       <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="55" t="s">
+      <c r="A34" s="57" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -6719,7 +7702,7 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
+      <c r="A35" s="58"/>
       <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
@@ -6734,7 +7717,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
+      <c r="A36" s="58"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -6749,7 +7732,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="3" t="s">
         <v>12</v>
       </c>
@@ -6764,7 +7747,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
+      <c r="A38" s="58"/>
       <c r="B38" s="3" t="s">
         <v>13</v>
       </c>
@@ -6779,8 +7762,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
-      <c r="B39" s="53" t="s">
+      <c r="A39" s="58"/>
+      <c r="B39" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -6795,8 +7778,8 @@
       <c r="F39" s="23"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="53"/>
+      <c r="A40" s="58"/>
+      <c r="B40" s="55"/>
       <c r="C40" s="16" t="s">
         <v>26</v>
       </c>
@@ -6809,8 +7792,8 @@
       <c r="F40" s="23"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="57"/>
-      <c r="B41" s="54"/>
+      <c r="A41" s="59"/>
+      <c r="B41" s="56"/>
       <c r="C41" s="17" t="s">
         <v>27</v>
       </c>
@@ -6823,7 +7806,7 @@
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="57" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -6839,7 +7822,7 @@
       <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="56"/>
+      <c r="A43" s="58"/>
       <c r="B43" s="3" t="s">
         <v>17</v>
       </c>
@@ -6852,7 +7835,7 @@
       <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
+      <c r="A44" s="58"/>
       <c r="B44" s="3" t="s">
         <v>11</v>
       </c>
@@ -6867,7 +7850,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
+      <c r="A45" s="58"/>
       <c r="B45" s="3" t="s">
         <v>12</v>
       </c>
@@ -6882,7 +7865,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
+      <c r="A46" s="58"/>
       <c r="B46" s="3" t="s">
         <v>13</v>
       </c>
@@ -6897,8 +7880,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
-      <c r="B47" s="53" t="s">
+      <c r="A47" s="58"/>
+      <c r="B47" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="16" t="s">
@@ -6913,8 +7896,8 @@
       <c r="F47" s="23"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="56"/>
-      <c r="B48" s="53"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="55"/>
       <c r="C48" s="16" t="s">
         <v>26</v>
       </c>
@@ -6927,8 +7910,8 @@
       <c r="F48" s="23"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="57"/>
-      <c r="B49" s="54"/>
+      <c r="A49" s="59"/>
+      <c r="B49" s="56"/>
       <c r="C49" s="17" t="s">
         <v>27</v>
       </c>
@@ -6941,7 +7924,7 @@
       <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="55" t="s">
+      <c r="A50" s="57" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -6957,7 +7940,7 @@
       <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
+      <c r="A51" s="58"/>
       <c r="B51" s="3" t="s">
         <v>17</v>
       </c>
@@ -6970,7 +7953,7 @@
       <c r="F51" s="23"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
+      <c r="A52" s="58"/>
       <c r="B52" s="3" t="s">
         <v>11</v>
       </c>
@@ -6983,7 +7966,7 @@
       <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="3" t="s">
         <v>12</v>
       </c>
@@ -6998,7 +7981,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
+      <c r="A54" s="58"/>
       <c r="B54" s="3" t="s">
         <v>13</v>
       </c>
@@ -7013,8 +7996,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
-      <c r="B55" s="53" t="s">
+      <c r="A55" s="58"/>
+      <c r="B55" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="16" t="s">
@@ -7029,8 +8012,8 @@
       <c r="F55" s="23"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="56"/>
-      <c r="B56" s="53"/>
+      <c r="A56" s="58"/>
+      <c r="B56" s="55"/>
       <c r="C56" s="16" t="s">
         <v>26</v>
       </c>
@@ -7043,8 +8026,8 @@
       <c r="F56" s="23"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="57"/>
-      <c r="B57" s="54"/>
+      <c r="A57" s="59"/>
+      <c r="B57" s="56"/>
       <c r="C57" s="17" t="s">
         <v>27</v>
       </c>
@@ -7057,11 +8040,11 @@
       <c r="F57" s="26"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="58" t="s">
+      <c r="A59" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="B59" s="58"/>
-      <c r="C59" s="59"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="54"/>
       <c r="D59" t="s">
         <v>160</v>
       </c>
@@ -7070,11 +8053,11 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="58" t="s">
+      <c r="A60" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="B60" s="58"/>
-      <c r="C60" s="59"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="54"/>
       <c r="D60" t="s">
         <v>162</v>
       </c>
@@ -7083,17 +8066,25 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="58"/>
-      <c r="B61" s="58"/>
-      <c r="C61" s="59"/>
+      <c r="A61" s="53"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="54"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="58"/>
-      <c r="B62" s="58"/>
-      <c r="C62" s="59"/>
+      <c r="A62" s="53"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
     <mergeCell ref="A59:C59"/>
     <mergeCell ref="A60:C60"/>
     <mergeCell ref="A61:C61"/>
@@ -7104,14 +8095,6 @@
     <mergeCell ref="A50:A57"/>
     <mergeCell ref="A42:A49"/>
     <mergeCell ref="A34:A41"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7122,8 +8105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA9E807-1B68-4F99-A999-3003C8845019}">
   <dimension ref="A2:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final additions for completeness
</commit_message>
<xml_diff>
--- a/Hypothesis and Results.xlsx
+++ b/Hypothesis and Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\University\General\UG4\SCC421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8980F2-89B8-45EF-B896-6344B0805E65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB73F592-905F-4DA2-93E8-91AD61F290E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5E275FB1-B708-4BF3-95EB-521DB5DA9B70}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -1513,12 +1513,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1533,6 +1527,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9780,7 +9780,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="56" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -9796,7 +9796,7 @@
       <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -9811,7 +9811,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
+      <c r="A4" s="57"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
@@ -9824,7 +9824,7 @@
       <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -9839,7 +9839,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="59"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -9854,8 +9854,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="56" t="s">
+      <c r="A7" s="57"/>
+      <c r="B7" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="16" t="s">
@@ -9870,8 +9870,8 @@
       <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="59"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
@@ -9884,8 +9884,8 @@
       <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="57"/>
+      <c r="A9" s="58"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="17" t="s">
         <v>27</v>
       </c>
@@ -9898,7 +9898,7 @@
       <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="56" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -9914,7 +9914,7 @@
       <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
@@ -9929,7 +9929,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -9944,7 +9944,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
@@ -9959,7 +9959,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
+      <c r="A14" s="57"/>
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
@@ -9974,8 +9974,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="56" t="s">
+      <c r="A15" s="57"/>
+      <c r="B15" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -9992,8 +9992,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="16" t="s">
         <v>26</v>
       </c>
@@ -10008,8 +10008,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
-      <c r="B17" s="57"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="17" t="s">
         <v>27</v>
       </c>
@@ -10022,7 +10022,7 @@
       <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="56" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -10038,7 +10038,7 @@
       <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
@@ -10053,7 +10053,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -10068,7 +10068,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
@@ -10083,7 +10083,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="3" t="s">
         <v>13</v>
       </c>
@@ -10096,8 +10096,8 @@
       <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="56" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="16" t="s">
@@ -10112,8 +10112,8 @@
       <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="56"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="16" t="s">
         <v>26</v>
       </c>
@@ -10126,8 +10126,8 @@
       <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
-      <c r="B25" s="57"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="55"/>
       <c r="C25" s="17" t="s">
         <v>27</v>
       </c>
@@ -10136,7 +10136,7 @@
       <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="56" t="s">
         <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -10152,7 +10152,7 @@
       <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
@@ -10165,7 +10165,7 @@
       <c r="F27" s="23"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -10180,7 +10180,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="3" t="s">
         <v>12</v>
       </c>
@@ -10195,7 +10195,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="59"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="3" t="s">
         <v>13</v>
       </c>
@@ -10208,8 +10208,8 @@
       <c r="F30" s="23"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
-      <c r="B31" s="56" t="s">
+      <c r="A31" s="57"/>
+      <c r="B31" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -10224,8 +10224,8 @@
       <c r="F31" s="23"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="16" t="s">
         <v>26</v>
       </c>
@@ -10238,8 +10238,8 @@
       <c r="F32" s="23"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="60"/>
-      <c r="B33" s="57"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="17" t="s">
         <v>27</v>
       </c>
@@ -10248,7 +10248,7 @@
       <c r="F33" s="26"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="56" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -10264,7 +10264,7 @@
       <c r="F34" s="23"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
+      <c r="A35" s="57"/>
       <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
@@ -10279,7 +10279,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
+      <c r="A36" s="57"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -10294,7 +10294,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
+      <c r="A37" s="57"/>
       <c r="B37" s="3" t="s">
         <v>12</v>
       </c>
@@ -10309,7 +10309,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
+      <c r="A38" s="57"/>
       <c r="B38" s="3" t="s">
         <v>13</v>
       </c>
@@ -10324,8 +10324,8 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="59"/>
-      <c r="B39" s="56" t="s">
+      <c r="A39" s="57"/>
+      <c r="B39" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="16" t="s">
@@ -10340,8 +10340,8 @@
       <c r="F39" s="23"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
-      <c r="B40" s="56"/>
+      <c r="A40" s="57"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="16" t="s">
         <v>26</v>
       </c>
@@ -10354,8 +10354,8 @@
       <c r="F40" s="23"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="60"/>
-      <c r="B41" s="57"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="55"/>
       <c r="C41" s="17" t="s">
         <v>27</v>
       </c>
@@ -10368,7 +10368,7 @@
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="56" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -10384,7 +10384,7 @@
       <c r="F42" s="23"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="59"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="3" t="s">
         <v>17</v>
       </c>
@@ -10397,7 +10397,7 @@
       <c r="F43" s="23"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
+      <c r="A44" s="57"/>
       <c r="B44" s="3" t="s">
         <v>11</v>
       </c>
@@ -10412,7 +10412,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
+      <c r="A45" s="57"/>
       <c r="B45" s="3" t="s">
         <v>12</v>
       </c>
@@ -10427,7 +10427,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
+      <c r="A46" s="57"/>
       <c r="B46" s="3" t="s">
         <v>13</v>
       </c>
@@ -10442,8 +10442,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="56" t="s">
+      <c r="A47" s="57"/>
+      <c r="B47" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="16" t="s">
@@ -10458,8 +10458,8 @@
       <c r="F47" s="23"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="59"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="57"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="16" t="s">
         <v>26</v>
       </c>
@@ -10472,8 +10472,8 @@
       <c r="F48" s="23"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="60"/>
-      <c r="B49" s="57"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="17" t="s">
         <v>27</v>
       </c>
@@ -10486,7 +10486,7 @@
       <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="56" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -10502,7 +10502,7 @@
       <c r="F50" s="23"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="59"/>
+      <c r="A51" s="57"/>
       <c r="B51" s="3" t="s">
         <v>17</v>
       </c>
@@ -10515,7 +10515,7 @@
       <c r="F51" s="23"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="59"/>
+      <c r="A52" s="57"/>
       <c r="B52" s="3" t="s">
         <v>11</v>
       </c>
@@ -10528,7 +10528,7 @@
       <c r="F52" s="23"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="59"/>
+      <c r="A53" s="57"/>
       <c r="B53" s="3" t="s">
         <v>12</v>
       </c>
@@ -10543,7 +10543,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="59"/>
+      <c r="A54" s="57"/>
       <c r="B54" s="3" t="s">
         <v>13</v>
       </c>
@@ -10558,8 +10558,8 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="59"/>
-      <c r="B55" s="56" t="s">
+      <c r="A55" s="57"/>
+      <c r="B55" s="54" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="16" t="s">
@@ -10574,8 +10574,8 @@
       <c r="F55" s="23"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="59"/>
-      <c r="B56" s="56"/>
+      <c r="A56" s="57"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="16" t="s">
         <v>26</v>
       </c>
@@ -10588,8 +10588,8 @@
       <c r="F56" s="23"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="60"/>
-      <c r="B57" s="57"/>
+      <c r="A57" s="58"/>
+      <c r="B57" s="55"/>
       <c r="C57" s="17" t="s">
         <v>27</v>
       </c>
@@ -10602,11 +10602,11 @@
       <c r="F57" s="26"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="54" t="s">
+      <c r="A59" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="B59" s="54"/>
-      <c r="C59" s="55"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="60"/>
       <c r="D59" t="s">
         <v>157</v>
       </c>
@@ -10615,11 +10615,11 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B60" s="54"/>
-      <c r="C60" s="55"/>
+      <c r="B60" s="59"/>
+      <c r="C60" s="60"/>
       <c r="D60" t="s">
         <v>159</v>
       </c>
@@ -10628,25 +10628,17 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="54"/>
-      <c r="B61" s="54"/>
-      <c r="C61" s="55"/>
+      <c r="A61" s="59"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="60"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="54"/>
-      <c r="B62" s="54"/>
-      <c r="C62" s="55"/>
+      <c r="A62" s="59"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A25"/>
     <mergeCell ref="A59:C59"/>
     <mergeCell ref="A60:C60"/>
     <mergeCell ref="A61:C61"/>
@@ -10657,6 +10649,14 @@
     <mergeCell ref="A50:A57"/>
     <mergeCell ref="A42:A49"/>
     <mergeCell ref="A34:A41"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11797,7 +11797,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>